<commit_message>
implement device status and sim card status
</commit_message>
<xml_diff>
--- a/Afaqy_Store/App_Data/SIMCard.xlsx
+++ b/Afaqy_Store/App_Data/SIMCard.xlsx
@@ -251,49 +251,32 @@
     <x:row r="15">
       <x:c r="A15" t="inlineStr">
         <x:is>
-          <x:t>14</x:t>
+          <x:t>15</x:t>
         </x:is>
       </x:c>
       <x:c r="B15" t="inlineStr">
         <x:is>
-          <x:t>136</x:t>
+          <x:t>1366</x:t>
         </x:is>
       </x:c>
       <x:c r="C15" t="inlineStr">
         <x:is>
-          <x:t>058</x:t>
+          <x:t>0588</x:t>
         </x:is>
       </x:c>
     </x:row>
     <x:row r="16">
       <x:c r="A16" t="inlineStr">
         <x:is>
-          <x:t>15</x:t>
+          <x:t>16</x:t>
         </x:is>
       </x:c>
       <x:c r="B16" t="inlineStr">
         <x:is>
-          <x:t>137</x:t>
+          <x:t>136</x:t>
         </x:is>
       </x:c>
       <x:c r="C16" t="inlineStr">
-        <x:is>
-          <x:t>058</x:t>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="17">
-      <x:c r="A17" t="inlineStr">
-        <x:is>
-          <x:t>65</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="B17" t="inlineStr">
-        <x:is>
-          <x:t>138</x:t>
-        </x:is>
-      </x:c>
-      <x:c r="C17" t="inlineStr">
         <x:is>
           <x:t>058</x:t>
         </x:is>

</xml_diff>